<commit_message>
added python3 scripts for adding quests about enchantments
</commit_message>
<xml_diff>
--- a/.workspace/shop/shoplist.xlsx
+++ b/.workspace/shop/shoplist.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="289">
   <si>
     <t>#ignore rows that start with a '#'</t>
   </si>
@@ -1022,10 +1022,6 @@
     </r>
   </si>
   <si>
-    <t>akashictome:tome {"akashictome:data":{tconstruct:{id:"tconstruct:book",Count:1b,tag:{"akashictome:definedMod":"tconstruct",mantle:{book:{page:"materials.palladium"}}},Damage:0s},conarm:{id:"conarm:book",Count:1b,tag:{"akashictome:definedMod":"conarm"},Damage:0s},ftbquests:{id:"ftbquests:book",Count:1b,tag:{"akashictome:definedMod":"ftbquests"},Damage:0s},extrautils2:{id:"extrautils2:book",Count:1b,tag:{"akashictome:definedMod":"extrautils2"},Damage:0s},immersiveengineering:{id:"immersiveengineering:tool",Count:1b,tag:{"akashictome:definedMod":"immersiveengineering"},Damage:3s},opencomputers:{id:"opencomputers:tool",Count:1b,tag:{"akashictome:definedMod":"opencomputers"},Damage:4s},iceandfire:{id:"iceandfire:bestiary",Count:1b,tag:{Pages:[I;0],"akashictome:definedMod":"iceandfire"},Damage:0s},ebwizardry:{id:"ebwizardry:wizard_handbook",Count:1b,tag:{"akashictome:definedMod":"ebwizardry"},Damage:0s}}}</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>s</t>
     </r>
@@ -1254,10 +1250,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>v1.99.6</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>minecraft:fireworks</t>
     </r>
@@ -1398,14 +1390,6 @@
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
-    <t>Dye</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ammo</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t>h</t>
     </r>
@@ -2184,6 +2168,178 @@
         <scheme val="minor"/>
       </rPr>
       <t>uy</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>sell</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ustic:slate</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uy</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ustic:log:0</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ustic:log:1</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2.0.6</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dye &amp; Ammo</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>Logs</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>#</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Logs</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>akashictome:tome {"akashictome:data":{tconstruct:{id:"tconstruct:book",Count:1b,tag:{"akashictome:definedMod":"tconstruct"},Damage:0s},rustic:{id:"rustic:book",Count:1b,tag:{"akashictome:definedMod":"rustic"},Damage:0s},mysticalworld:{id:"patchouli:guide_book",Count:1b,tag:{"akashictome:definedMod":"mysticalworld","patchouli:book":"mysticalworld:world_guide"},Damage:0s},conarm:{id:"conarm:book",Count:1b,tag:{"akashictome:definedMod":"conarm"},Damage:0s},extrautils2:{id:"extrautils2:book",Count:1b,tag:{"akashictome:definedMod":"extrautils2"},Damage:0s},ftbquests:{id:"ftbquests:book",Count:1b,tag:{"akashictome:definedMod":"ftbquests"},Damage:0s},immersiveengineering:{id:"immersiveengineering:tool",Count:1b,tag:{"akashictome:definedMod":"immersiveengineering"},Damage:3s},roots:{id:"patchouli:guide_book",Count:1b,tag:{"akashictome:definedMod":"roots","patchouli:book":"roots:roots_guide"},Damage:0s},cookingforblockheads:{id:"cookingforblockheads:recipe_book",Count:1b,tag:{"akashictome:definedMod":"cookingforblockheads"},Damage:1s},iceandfire:{id:"iceandfire:bestiary",Count:1b,tag:{"akashictome:definedMod":"iceandfire"},Damage:0s},openblocks:{id:"openblocks:info_book",Count:1b,tag:{"akashictome:definedMod":"openblocks"},Damage:0s},ebwizardry:{id:"ebwizardry:wizard_handbook",Count:1b,tag:{"akashictome:definedMod":"ebwizardry"},Damage:0s}}}</t>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uy</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inecraft:dirt</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>b</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>uy</t>
+    </r>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>m</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inecraft:cobble_stone</t>
     </r>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -2405,7 +2561,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
@@ -2430,28 +2586,28 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
@@ -2460,16 +2616,38 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
@@ -2478,35 +2656,22 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1">
@@ -2515,16 +2680,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2810,8 +2972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2820,7 +2982,8 @@
     <col min="2" max="2" width="13.5546875" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.44140625" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.88671875" style="7"/>
+    <col min="5" max="5" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="7"/>
     <col min="7" max="7" width="17.77734375" style="7" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="7"/>
   </cols>
@@ -2914,10 +3077,10 @@
         <v>43</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>192</v>
+        <v>281</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>193</v>
+        <v>282</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>151</v>
@@ -2930,11 +3093,11 @@
       <c r="B11" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>244</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>245</v>
+      <c r="C11" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>241</v>
       </c>
       <c r="E11" s="12"/>
     </row>
@@ -2943,11 +3106,11 @@
         <v>150</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>175</v>
+        <v>280</v>
       </c>
       <c r="C13" s="3">
         <f ca="1">TODAY()</f>
-        <v>43819</v>
+        <v>43836</v>
       </c>
     </row>
   </sheetData>
@@ -2959,10 +3122,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D217"/>
+  <dimension ref="A1:D216"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3008,11 +3171,11 @@
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="34" t="s">
-        <v>237</v>
-      </c>
-      <c r="B5" s="34" t="s">
-        <v>236</v>
+      <c r="A5" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>232</v>
       </c>
       <c r="C5" s="9">
         <v>250</v>
@@ -3022,11 +3185,11 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="41" t="s">
-        <v>278</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>277</v>
+      <c r="A6" s="39" t="s">
+        <v>274</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>273</v>
       </c>
       <c r="C6" s="9">
         <v>50</v>
@@ -3036,12 +3199,32 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="24"/>
-      <c r="B8" s="25"/>
+      <c r="A8" s="44" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="9" t="s">
@@ -3091,11 +3274,11 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>241</v>
+      <c r="A14" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>237</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
@@ -3105,11 +3288,11 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="B15" s="35" t="s">
-        <v>243</v>
+      <c r="A15" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>239</v>
       </c>
       <c r="C15" s="9">
         <v>1.25</v>
@@ -3217,599 +3400,631 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="9">
-        <v>7.5</v>
+      <c r="A23" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" s="1">
+        <v>2</v>
       </c>
       <c r="D23" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C24" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D24" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="C25" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D25" s="9">
-        <v>1</v>
-      </c>
-    </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C26" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D26" s="9">
+      <c r="A26" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="14">
+        <v>200</v>
+      </c>
+      <c r="D26" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C27" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D27" s="9">
+      <c r="A27" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="14">
+        <v>200</v>
+      </c>
+      <c r="D27" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="C28" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D28" s="9">
+      <c r="A28" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="14">
+        <v>200</v>
+      </c>
+      <c r="D28" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D29" s="9">
+      <c r="A29" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="C29" s="14">
+        <v>200</v>
+      </c>
+      <c r="D29" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D30" s="9">
+      <c r="A30" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" s="14">
+        <v>200</v>
+      </c>
+      <c r="D30" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="C31" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D31" s="9">
+      <c r="A31" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C31" s="14">
+        <v>200</v>
+      </c>
+      <c r="D31" s="14">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D32" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="C33" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D33" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="C35" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="C36" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D36" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="C37" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D37" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C38" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D38" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D39" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C40" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D40" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D41" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D42" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="C43" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D43" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="C44" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D44" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D45" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D46" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D47" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="C48" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D48" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D49" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="41" t="s">
-        <v>265</v>
-      </c>
-      <c r="C50" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D50" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="41" t="s">
-        <v>266</v>
-      </c>
-      <c r="C51" s="9">
-        <v>7.5</v>
-      </c>
-      <c r="D51" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="23"/>
-      <c r="B52" s="13"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="23"/>
-      <c r="B53" s="13"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="23"/>
-      <c r="B54" s="13"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="23"/>
-      <c r="B55" s="13"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="23"/>
-      <c r="B56" s="13"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="23"/>
-      <c r="B57" s="13"/>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C60" s="15">
-        <v>200</v>
-      </c>
-      <c r="D60" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C61" s="15">
-        <v>200</v>
-      </c>
-      <c r="D61" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C62" s="15">
-        <v>200</v>
-      </c>
-      <c r="D62" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C63" s="15">
-        <v>200</v>
-      </c>
-      <c r="D63" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C64" s="15">
-        <v>200</v>
-      </c>
-      <c r="D64" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C65" s="15">
-        <v>200</v>
-      </c>
-      <c r="D65" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="23"/>
-      <c r="B66" s="23"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="23"/>
-      <c r="B67" s="23"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="34"/>
-      <c r="B68" s="23"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="23"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="23"/>
-    </row>
-    <row r="71" spans="1:4">
-      <c r="A71" s="23"/>
+      <c r="A32" s="22"/>
+      <c r="B32" s="22"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="32"/>
+      <c r="B34" s="22"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="22"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="22"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="22"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="22"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="22"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="22"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="22"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="22"/>
+      <c r="B42" s="22"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="22"/>
+      <c r="B47" s="22"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="22"/>
+      <c r="B48" s="22"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="22"/>
+      <c r="B49" s="22"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="23"/>
+      <c r="A72" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="23"/>
+      <c r="A73" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B73" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C73" s="9">
+        <v>6</v>
+      </c>
+      <c r="D73" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="23"/>
+      <c r="A74" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="9">
+        <v>6</v>
+      </c>
+      <c r="D74" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="23"/>
+      <c r="A75" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C75" s="9">
+        <v>6</v>
+      </c>
+      <c r="D75" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="23"/>
-      <c r="B76" s="23"/>
+      <c r="A76" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C76" s="9">
+        <v>6</v>
+      </c>
+      <c r="D76" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="23"/>
-      <c r="B77" s="23"/>
+      <c r="A77" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="9">
+        <v>6</v>
+      </c>
+      <c r="D77" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="23"/>
-      <c r="B78" s="23"/>
+      <c r="A78" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C78" s="9">
+        <v>6</v>
+      </c>
+      <c r="D78" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="79" spans="1:4">
-      <c r="A79" s="23"/>
-      <c r="B79" s="23"/>
+      <c r="A79" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="9">
+        <v>6</v>
+      </c>
+      <c r="D79" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="23"/>
-      <c r="B80" s="23"/>
-    </row>
-    <row r="81" spans="1:2">
-      <c r="A81" s="23"/>
-      <c r="B81" s="23"/>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="23"/>
-      <c r="B82" s="23"/>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="23"/>
-      <c r="B83" s="23"/>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" s="23"/>
-      <c r="B84" s="23"/>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="9" t="s">
-        <v>44</v>
+      <c r="A80" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="9">
+        <v>6</v>
+      </c>
+      <c r="D80" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" s="9">
+        <v>6</v>
+      </c>
+      <c r="D81" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C82" s="9">
+        <v>6</v>
+      </c>
+      <c r="D82" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" s="9">
+        <v>6</v>
+      </c>
+      <c r="D83" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" s="9">
+        <v>6</v>
+      </c>
+      <c r="D84" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C85" s="9">
+        <v>6</v>
+      </c>
+      <c r="D85" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C86" s="9">
+        <v>6</v>
+      </c>
+      <c r="D86" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87" s="9">
+        <v>6</v>
+      </c>
+      <c r="D87" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B88" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C88" s="9">
+        <v>6</v>
+      </c>
+      <c r="D88" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C90" s="9">
+        <v>6</v>
+      </c>
+      <c r="D90" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C91" s="9">
+        <v>6</v>
+      </c>
+      <c r="D91" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C92" s="9">
+        <v>6</v>
+      </c>
+      <c r="D92" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B93" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C93" s="9">
+        <v>6</v>
+      </c>
+      <c r="D93" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" s="9">
+        <v>6</v>
+      </c>
+      <c r="D94" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C95" s="9">
+        <v>6</v>
+      </c>
+      <c r="D95" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C96" s="9">
+        <v>6</v>
+      </c>
+      <c r="D96" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C97" s="9">
+        <v>6</v>
+      </c>
+      <c r="D97" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C98" s="9">
+        <v>6</v>
+      </c>
+      <c r="D98" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C99" s="9">
+        <v>6</v>
+      </c>
+      <c r="D99" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B100" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C100" s="9">
+        <v>6</v>
+      </c>
+      <c r="D100" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="9">
+        <v>6</v>
+      </c>
+      <c r="D101" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C102" s="9">
+        <v>6</v>
+      </c>
+      <c r="D102" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C103" s="9">
+        <v>6</v>
+      </c>
+      <c r="D103" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C104" s="9">
+        <v>6</v>
+      </c>
+      <c r="D104" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C105" s="9">
+        <v>6</v>
+      </c>
+      <c r="D105" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="C107" s="9">
         <v>6</v>
@@ -3823,7 +4038,7 @@
         <v>12</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C108" s="9">
         <v>6</v>
@@ -3834,10 +4049,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="C109" s="9">
         <v>6</v>
@@ -3851,7 +4066,7 @@
         <v>12</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="C110" s="9">
         <v>6</v>
@@ -3862,10 +4077,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="C111" s="9">
         <v>6</v>
@@ -3879,7 +4094,7 @@
         <v>12</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C112" s="9">
         <v>6</v>
@@ -3890,10 +4105,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C113" s="9">
         <v>6</v>
@@ -3907,7 +4122,7 @@
         <v>12</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C114" s="9">
         <v>6</v>
@@ -3918,10 +4133,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C115" s="9">
         <v>6</v>
@@ -3935,7 +4150,7 @@
         <v>12</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="C116" s="9">
         <v>6</v>
@@ -3946,10 +4161,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C117" s="9">
         <v>6</v>
@@ -3963,7 +4178,7 @@
         <v>12</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="C118" s="9">
         <v>6</v>
@@ -3974,10 +4189,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="C119" s="9">
         <v>6</v>
@@ -3991,7 +4206,7 @@
         <v>12</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C120" s="9">
         <v>6</v>
@@ -4002,10 +4217,10 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="9" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="C121" s="9">
         <v>6</v>
@@ -4019,7 +4234,7 @@
         <v>12</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="C122" s="9">
         <v>6</v>
@@ -4028,697 +4243,707 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C124" s="9">
-        <v>6</v>
-      </c>
-      <c r="D124" s="9">
-        <v>2</v>
-      </c>
-    </row>
     <row r="125" spans="1:4">
       <c r="A125" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C125" s="9">
-        <v>6</v>
-      </c>
-      <c r="D125" s="9">
-        <v>2</v>
+        <v>77</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="C126" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D126" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="C127" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D127" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C128" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D128" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C129" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D129" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="C130" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D130" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="C131" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D131" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="C132" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D132" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="C133" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D133" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="C134" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D134" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C135" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D135" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="9" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="C136" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D136" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C137" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D137" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>59</v>
+        <v>86</v>
       </c>
       <c r="C138" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D138" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="9" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B139" s="9" t="s">
-        <v>60</v>
+        <v>87</v>
       </c>
       <c r="C139" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D139" s="9">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C140" s="9">
+        <v>1</v>
+      </c>
+      <c r="D140" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:4">
       <c r="A141" s="9" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="C141" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D141" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4">
-      <c r="A142" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B142" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C142" s="9">
-        <v>6</v>
-      </c>
-      <c r="D142" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B143" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C143" s="9">
-        <v>6</v>
-      </c>
-      <c r="D143" s="9">
-        <v>2</v>
+      <c r="A143" s="13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B144" s="9" t="s">
-        <v>64</v>
+      <c r="A144" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B144" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="C144" s="9">
-        <v>6</v>
+        <v>1.4</v>
       </c>
       <c r="D144" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B145" s="9" t="s">
-        <v>65</v>
+      <c r="A145" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B145" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="C145" s="9">
-        <v>6</v>
+        <v>0.5</v>
       </c>
       <c r="D145" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:4">
-      <c r="A146" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B146" s="9" t="s">
-        <v>66</v>
+      <c r="A146" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B146" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="C146" s="9">
-        <v>6</v>
+        <v>1.3</v>
       </c>
       <c r="D146" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>67</v>
+      <c r="A147" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B147" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="C147" s="9">
-        <v>6</v>
+        <v>1.3</v>
       </c>
       <c r="D147" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B148" s="9" t="s">
-        <v>68</v>
+      <c r="A148" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B148" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="C148" s="9">
-        <v>6</v>
+        <v>3.3</v>
       </c>
       <c r="D148" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B149" s="9" t="s">
-        <v>69</v>
+      <c r="A149" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B149" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="C149" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D149" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:4">
-      <c r="A150" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B150" s="9" t="s">
-        <v>70</v>
+      <c r="A150" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B150" s="17" t="s">
+        <v>172</v>
       </c>
       <c r="C150" s="9">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D150" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B151" s="9" t="s">
-        <v>71</v>
+      <c r="A151" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B151" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="C151" s="9">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D151" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:4">
-      <c r="A152" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B152" s="9" t="s">
-        <v>72</v>
+      <c r="A152" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="C152" s="9">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D152" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B153" s="9" t="s">
-        <v>73</v>
+      <c r="A153" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B153" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="C153" s="9">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="D153" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="1:4">
-      <c r="A154" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B154" s="9" t="s">
-        <v>74</v>
+      <c r="A154" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B154" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="C154" s="9">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D154" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155" spans="1:4">
-      <c r="A155" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B155" s="9" t="s">
-        <v>75</v>
+      <c r="A155" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B155" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="C155" s="9">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D155" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="156" spans="1:4">
-      <c r="A156" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B156" s="9" t="s">
-        <v>76</v>
+      <c r="A156" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B156" s="18" t="s">
+        <v>179</v>
       </c>
       <c r="C156" s="9">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D156" s="9">
-        <v>2</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B157" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="C157" s="9">
+        <v>30</v>
+      </c>
+      <c r="D157" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B158" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="C158" s="9">
+        <v>25</v>
+      </c>
+      <c r="D158" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="159" spans="1:4">
-      <c r="A159" s="9" t="s">
-        <v>77</v>
+      <c r="A159" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B159" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="C159" s="9">
+        <v>27</v>
+      </c>
+      <c r="D159" s="9">
+        <v>3</v>
       </c>
     </row>
     <row r="160" spans="1:4">
-      <c r="A160" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B160" s="9" t="s">
-        <v>90</v>
+      <c r="A160" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B160" s="18" t="s">
+        <v>183</v>
       </c>
       <c r="C160" s="9">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D160" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4">
-      <c r="A161" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B161" s="9" t="s">
-        <v>91</v>
+      <c r="A161" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B161" s="18" t="s">
+        <v>184</v>
       </c>
       <c r="C161" s="9">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="D161" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B162" s="9" t="s">
-        <v>92</v>
+      <c r="A162" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B162" s="18" t="s">
+        <v>185</v>
       </c>
       <c r="C162" s="9">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D162" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B163" s="9" t="s">
-        <v>93</v>
+      <c r="A163" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B163" s="18" t="s">
+        <v>186</v>
       </c>
       <c r="C163" s="9">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D163" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:4">
-      <c r="A164" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B164" s="9" t="s">
-        <v>94</v>
+      <c r="A164" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B164" s="18" t="s">
+        <v>187</v>
       </c>
       <c r="C164" s="9">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D164" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B165" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C165" s="9">
-        <v>1</v>
-      </c>
-      <c r="D165" s="9">
-        <v>3</v>
-      </c>
+      <c r="A165" s="18"/>
+      <c r="B165" s="18"/>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B166" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C166" s="9">
-        <v>1</v>
-      </c>
-      <c r="D166" s="9">
-        <v>3</v>
-      </c>
+      <c r="A166" s="43" t="s">
+        <v>283</v>
+      </c>
+      <c r="B166" s="18"/>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B167" s="9" t="s">
-        <v>81</v>
+      <c r="A167" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>122</v>
       </c>
       <c r="C167" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D167" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B168" s="9" t="s">
-        <v>82</v>
+      <c r="A168" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B168" s="13" t="s">
+        <v>123</v>
       </c>
       <c r="C168" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D168" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B169" s="9" t="s">
-        <v>83</v>
+      <c r="A169" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B169" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="C169" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D169" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>84</v>
+      <c r="A170" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B170" s="13" t="s">
+        <v>125</v>
       </c>
       <c r="C170" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D170" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>85</v>
+      <c r="A171" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B171" s="13" t="s">
+        <v>126</v>
       </c>
       <c r="C171" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D171" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B172" s="9" t="s">
-        <v>86</v>
+      <c r="A172" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B172" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="C172" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D172" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B173" s="9" t="s">
-        <v>87</v>
+      <c r="A173" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B173" s="13" t="s">
+        <v>128</v>
       </c>
       <c r="C173" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D173" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B174" s="9" t="s">
-        <v>88</v>
+      <c r="A174" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B174" s="13" t="s">
+        <v>129</v>
       </c>
       <c r="C174" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D174" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="175" spans="1:4">
-      <c r="A175" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B175" s="9" t="s">
-        <v>89</v>
+      <c r="A175" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B175" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="C175" s="9">
-        <v>1</v>
+        <v>7.5</v>
       </c>
       <c r="D175" s="9">
-        <v>3</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B176" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C176" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="D176" s="9">
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:4">
       <c r="A177" s="13" t="s">
-        <v>99</v>
+        <v>117</v>
+      </c>
+      <c r="B177" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C177" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="D177" s="9">
+        <v>4</v>
       </c>
     </row>
     <row r="178" spans="1:4">
       <c r="A178" s="13" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B178" s="13" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C178" s="9">
-        <v>1.4</v>
+        <v>7.5</v>
       </c>
       <c r="D178" s="9">
         <v>4</v>
@@ -4726,13 +4951,13 @@
     </row>
     <row r="179" spans="1:4">
       <c r="A179" s="13" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B179" s="13" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="C179" s="9">
-        <v>0.5</v>
+        <v>7.5</v>
       </c>
       <c r="D179" s="9">
         <v>4</v>
@@ -4740,13 +4965,13 @@
     </row>
     <row r="180" spans="1:4">
       <c r="A180" s="13" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B180" s="13" t="s">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="C180" s="9">
-        <v>1.3</v>
+        <v>7.5</v>
       </c>
       <c r="D180" s="9">
         <v>4</v>
@@ -4754,13 +4979,13 @@
     </row>
     <row r="181" spans="1:4">
       <c r="A181" s="13" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B181" s="13" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="C181" s="9">
-        <v>1.3</v>
+        <v>7.5</v>
       </c>
       <c r="D181" s="9">
         <v>4</v>
@@ -4768,257 +4993,257 @@
     </row>
     <row r="182" spans="1:4">
       <c r="A182" s="13" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B182" s="13" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="C182" s="9">
-        <v>3.3</v>
+        <v>7.5</v>
       </c>
       <c r="D182" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:4">
-      <c r="A183" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B183" s="18" t="s">
-        <v>172</v>
+      <c r="A183" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B183" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="C183" s="9">
-        <v>2</v>
+        <v>7.5</v>
       </c>
       <c r="D183" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="184" spans="1:4">
-      <c r="A184" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B184" s="18" t="s">
-        <v>173</v>
+      <c r="A184" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B184" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="C184" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D184" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="185" spans="1:4">
-      <c r="A185" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B185" s="19" t="s">
-        <v>177</v>
+      <c r="A185" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B185" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="C185" s="9">
-        <v>75</v>
+        <v>7.5</v>
       </c>
       <c r="D185" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="186" spans="1:4">
-      <c r="A186" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B186" s="19" t="s">
-        <v>178</v>
+      <c r="A186" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B186" s="13" t="s">
+        <v>141</v>
       </c>
       <c r="C186" s="9">
-        <v>75</v>
+        <v>7.5</v>
       </c>
       <c r="D186" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="187" spans="1:4">
-      <c r="A187" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B187" s="19" t="s">
-        <v>176</v>
+      <c r="A187" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B187" s="13" t="s">
+        <v>142</v>
       </c>
       <c r="C187" s="9">
-        <v>75</v>
+        <v>7.5</v>
       </c>
       <c r="D187" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="188" spans="1:4">
-      <c r="A188" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B188" s="19" t="s">
-        <v>179</v>
+      <c r="A188" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B188" s="13" t="s">
+        <v>143</v>
       </c>
       <c r="C188" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D188" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="189" spans="1:4">
-      <c r="A189" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B189" s="19" t="s">
-        <v>180</v>
+      <c r="A189" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B189" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="C189" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D189" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="190" spans="1:4">
-      <c r="A190" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B190" s="19" t="s">
-        <v>181</v>
+      <c r="A190" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B190" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="C190" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D190" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="191" spans="1:4">
-      <c r="A191" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B191" s="19" t="s">
-        <v>182</v>
+      <c r="A191" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B191" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="C191" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D191" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="192" spans="1:4">
-      <c r="A192" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B192" s="19" t="s">
-        <v>183</v>
+      <c r="A192" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B192" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="C192" s="9">
-        <v>25</v>
+        <v>7.5</v>
       </c>
       <c r="D192" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="193" spans="1:4">
-      <c r="A193" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B193" s="19" t="s">
-        <v>184</v>
+      <c r="A193" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B193" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="C193" s="9">
-        <v>27</v>
+        <v>7.5</v>
       </c>
       <c r="D193" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="194" spans="1:4">
-      <c r="A194" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B194" s="19" t="s">
-        <v>185</v>
+      <c r="A194" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B194" s="39" t="s">
+        <v>261</v>
       </c>
       <c r="C194" s="9">
-        <v>27</v>
+        <v>7.5</v>
       </c>
       <c r="D194" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="195" spans="1:4">
-      <c r="A195" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B195" s="19" t="s">
-        <v>186</v>
+      <c r="A195" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B195" s="39" t="s">
+        <v>262</v>
       </c>
       <c r="C195" s="9">
-        <v>150</v>
+        <v>7.5</v>
       </c>
       <c r="D195" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="196" spans="1:4">
-      <c r="A196" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B196" s="19" t="s">
-        <v>187</v>
+      <c r="A196" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="B196" s="42" t="s">
+        <v>278</v>
       </c>
       <c r="C196" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D196" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="197" spans="1:4">
-      <c r="A197" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B197" s="19" t="s">
-        <v>188</v>
+      <c r="A197" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="B197" s="42" t="s">
+        <v>279</v>
       </c>
       <c r="C197" s="9">
-        <v>30</v>
+        <v>7.5</v>
       </c>
       <c r="D197" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:4">
-      <c r="A198" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="B198" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C198" s="9">
-        <v>25</v>
-      </c>
-      <c r="D198" s="9">
-        <v>4</v>
-      </c>
+      <c r="A198" s="13"/>
+      <c r="B198" s="13"/>
     </row>
     <row r="199" spans="1:4">
-      <c r="A199" s="13"/>
-      <c r="B199" s="13"/>
+      <c r="A199" s="13" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="200" spans="1:4">
-      <c r="A200" s="13" t="s">
-        <v>119</v>
+      <c r="A200" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B200" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C200" s="9">
+        <v>30000</v>
+      </c>
+      <c r="D200" s="9">
+        <v>5</v>
       </c>
     </row>
     <row r="201" spans="1:4">
-      <c r="A201" s="34" t="s">
-        <v>238</v>
+      <c r="A201" s="32" t="s">
+        <v>234</v>
       </c>
       <c r="B201" s="13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C201" s="9">
         <v>30000</v>
@@ -5028,166 +5253,152 @@
       </c>
     </row>
     <row r="202" spans="1:4">
-      <c r="A202" s="34" t="s">
-        <v>238</v>
+      <c r="A202" s="32" t="s">
+        <v>234</v>
       </c>
       <c r="B202" s="13" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="C202" s="9">
-        <v>30000</v>
+        <v>60</v>
       </c>
       <c r="D202" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:4">
-      <c r="A203" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B203" s="13" t="s">
-        <v>149</v>
+      <c r="A203" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B203" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="C203" s="9">
-        <v>60</v>
-      </c>
-      <c r="D203" s="9">
+        <v>80000</v>
+      </c>
+      <c r="D203" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:4">
-      <c r="A204" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B204" s="16" t="s">
-        <v>152</v>
+      <c r="A204" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B204" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="C204" s="9">
-        <v>80000</v>
+        <v>20000</v>
       </c>
       <c r="D204" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:4">
-      <c r="A205" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B205" s="16" t="s">
-        <v>154</v>
+      <c r="A205" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B205" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="C205" s="9">
-        <v>20000</v>
+        <v>50000</v>
       </c>
       <c r="D205" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:4">
-      <c r="A206" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B206" s="16" t="s">
-        <v>155</v>
+      <c r="A206" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B206" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="C206" s="9">
-        <v>50000</v>
+        <v>250</v>
       </c>
       <c r="D206" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:4">
-      <c r="A207" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B207" s="16" t="s">
-        <v>156</v>
+      <c r="A207" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B207" s="15" t="s">
+        <v>157</v>
       </c>
       <c r="C207" s="9">
-        <v>250</v>
+        <v>750</v>
       </c>
       <c r="D207" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="208" spans="1:4">
-      <c r="A208" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B208" s="16" t="s">
-        <v>157</v>
+      <c r="A208" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B208" s="43" t="s">
+        <v>284</v>
       </c>
       <c r="C208" s="9">
-        <v>750</v>
+        <v>100</v>
       </c>
       <c r="D208" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="209" spans="1:4">
-      <c r="A209" s="34" t="s">
-        <v>239</v>
+      <c r="A209" s="32" t="s">
+        <v>234</v>
       </c>
       <c r="B209" s="14" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C209" s="9">
-        <v>100</v>
-      </c>
-      <c r="D209" s="10">
+        <v>300</v>
+      </c>
+      <c r="D209" s="9">
         <v>5</v>
       </c>
     </row>
     <row r="210" spans="1:4">
-      <c r="A210" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B210" s="15" t="s">
-        <v>168</v>
+      <c r="A210" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="B210" s="23" t="s">
+        <v>229</v>
       </c>
       <c r="C210" s="9">
-        <v>300</v>
+        <v>1000000</v>
       </c>
       <c r="D210" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
-      <c r="A211" s="34" t="s">
-        <v>238</v>
-      </c>
-      <c r="B211" s="25" t="s">
-        <v>233</v>
-      </c>
-      <c r="C211" s="9">
-        <v>1000000</v>
-      </c>
-      <c r="D211" s="9">
+    <row r="212" spans="1:4">
+      <c r="A212" s="17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4">
+      <c r="A213" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B213" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C213" s="9">
+        <v>32768</v>
+      </c>
+      <c r="D213" s="9">
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
-      <c r="A213" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4">
-      <c r="A214" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="B214" s="20" t="s">
-        <v>191</v>
-      </c>
-      <c r="C214" s="9">
-        <v>32768</v>
-      </c>
-      <c r="D214" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4">
-      <c r="B217" s="19"/>
+    <row r="216" spans="1:4">
+      <c r="B216" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
@@ -5200,8 +5411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -5247,11 +5458,11 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1">
-      <c r="A4" s="33" t="s">
-        <v>235</v>
-      </c>
-      <c r="B4" s="34" t="s">
-        <v>236</v>
+      <c r="A4" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>232</v>
       </c>
       <c r="C4" s="9">
         <v>250</v>
@@ -5261,11 +5472,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="9" customFormat="1">
-      <c r="A5" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>277</v>
+      <c r="A5" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>273</v>
       </c>
       <c r="C5" s="9">
         <v>50</v>
@@ -5275,24 +5486,44 @@
       </c>
     </row>
     <row r="6" spans="1:4" s="9" customFormat="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="9" customFormat="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="37" t="s">
-        <v>246</v>
+      <c r="A9" s="35" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>248</v>
+      <c r="A10" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>244</v>
       </c>
       <c r="C10" s="1">
         <v>3</v>
@@ -5302,39 +5533,39 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="35" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="35" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>248</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="35" t="s">
         <v>249</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B13" s="35" t="s">
         <v>250</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="37" t="s">
-        <v>251</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>252</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="37" t="s">
-        <v>253</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>254</v>
       </c>
       <c r="C13" s="1">
         <v>50</v>
@@ -5344,11 +5575,11 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>255</v>
+      <c r="A14" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>251</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -5358,11 +5589,11 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B15" s="42" t="s">
-        <v>267</v>
+      <c r="A15" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>263</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -5372,11 +5603,11 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>257</v>
+      <c r="A16" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>253</v>
       </c>
       <c r="C16" s="1">
         <v>6</v>
@@ -5386,11 +5617,11 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>258</v>
+      <c r="A17" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>254</v>
       </c>
       <c r="C17" s="1">
         <v>13.5</v>
@@ -5400,67 +5631,67 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>267</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B21" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="C21" s="1">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B22" s="40" t="s">
         <v>269</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="B19" s="42" t="s">
-        <v>270</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>271</v>
-      </c>
-      <c r="C20" s="1">
-        <v>2</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="B21" s="42" t="s">
-        <v>272</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>273</v>
       </c>
       <c r="C22" s="1">
         <v>5</v>
@@ -5470,11 +5701,11 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>274</v>
+      <c r="A23" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>270</v>
       </c>
       <c r="C23" s="1">
         <v>5</v>
@@ -5484,11 +5715,11 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="42" t="s">
-        <v>268</v>
-      </c>
-      <c r="B24" s="42" t="s">
-        <v>275</v>
+      <c r="A24" s="40" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>271</v>
       </c>
       <c r="C24" s="1">
         <v>5</v>
@@ -5504,19 +5735,19 @@
       <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="40" t="s">
-        <v>261</v>
+      <c r="A26" s="38" t="s">
+        <v>257</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B27" s="39" t="s">
-        <v>259</v>
+      <c r="A27" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>255</v>
       </c>
       <c r="C27" s="9">
         <v>6</v>
@@ -5526,11 +5757,11 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B28" s="38" t="s">
         <v>256</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>260</v>
       </c>
       <c r="C28" s="9">
         <v>5</v>
@@ -5540,8 +5771,8 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="38" t="s">
-        <v>256</v>
+      <c r="A29" s="36" t="s">
+        <v>252</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>13</v>
@@ -5554,8 +5785,8 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="38" t="s">
-        <v>256</v>
+      <c r="A30" s="36" t="s">
+        <v>252</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>15</v>
@@ -5568,8 +5799,8 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="38" t="s">
-        <v>256</v>
+      <c r="A31" s="36" t="s">
+        <v>252</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>17</v>
@@ -5582,11 +5813,11 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="38" t="s">
-        <v>256</v>
-      </c>
-      <c r="B32" s="40" t="s">
-        <v>262</v>
+      <c r="A32" s="36" t="s">
+        <v>252</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>258</v>
       </c>
       <c r="C32" s="9">
         <v>7</v>
@@ -5597,10 +5828,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="C33" s="1">
         <v>25</v>
@@ -5613,8 +5844,8 @@
       <c r="A34" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="40" t="s">
-        <v>263</v>
+      <c r="B34" s="38" t="s">
+        <v>259</v>
       </c>
       <c r="C34" s="9">
         <v>10</v>
@@ -5627,8 +5858,8 @@
       <c r="A35" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="40" t="s">
-        <v>264</v>
+      <c r="B35" s="38" t="s">
+        <v>260</v>
       </c>
       <c r="C35" s="9">
         <v>0.2</v>
@@ -5638,16 +5869,26 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="11"/>
-      <c r="B36" s="21"/>
+      <c r="A36" s="41" t="s">
+        <v>275</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>276</v>
+      </c>
+      <c r="C36" s="1">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="11"/>
-      <c r="B37" s="21"/>
+      <c r="B37" s="20"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="17"/>
-      <c r="B38" s="17"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
     </row>
     <row r="39" spans="1:4">
       <c r="C39" s="9"/>
@@ -5657,7 +5898,7 @@
       <c r="A40" s="11"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="B42" s="22"/>
+      <c r="B42" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="21" type="noConversion"/>
@@ -5685,53 +5926,53 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" t="s">
         <v>196</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G2" t="s">
         <v>197</v>
-      </c>
-      <c r="C2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s">
-        <v>200</v>
-      </c>
-      <c r="F2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="24" t="s">
         <v>109</v>
       </c>
       <c r="B5">
@@ -5749,8 +5990,8 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="26" t="s">
-        <v>194</v>
+      <c r="A6" s="24" t="s">
+        <v>190</v>
       </c>
       <c r="B6">
         <v>16</v>
@@ -5857,8 +6098,8 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="28" t="s">
-        <v>212</v>
+      <c r="A12" s="26" t="s">
+        <v>208</v>
       </c>
       <c r="E12" t="e">
         <f t="shared" si="0"/>
@@ -5866,8 +6107,8 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="29" t="s">
-        <v>214</v>
+      <c r="A13" s="27" t="s">
+        <v>210</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -5884,8 +6125,8 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="29" t="s">
-        <v>222</v>
+      <c r="A14" s="27" t="s">
+        <v>218</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -5901,12 +6142,12 @@
         <v>133</v>
       </c>
       <c r="G14" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="29" t="s">
-        <v>224</v>
+      <c r="A15" s="27" t="s">
+        <v>220</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -5922,12 +6163,12 @@
         <v>266</v>
       </c>
       <c r="G15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="29" t="s">
-        <v>223</v>
+      <c r="A16" s="27" t="s">
+        <v>219</v>
       </c>
       <c r="B16">
         <v>5</v>
@@ -5943,12 +6184,12 @@
         <v>300</v>
       </c>
       <c r="G16" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="29" t="s">
-        <v>220</v>
+      <c r="A17" s="27" t="s">
+        <v>216</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -5964,12 +6205,12 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="29" t="s">
-        <v>225</v>
+      <c r="A18" s="27" t="s">
+        <v>221</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -5985,12 +6226,12 @@
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="29" t="s">
-        <v>226</v>
+      <c r="A19" s="27" t="s">
+        <v>222</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -6006,7 +6247,7 @@
         <v>50</v>
       </c>
       <c r="G19" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -6027,12 +6268,12 @@
         <v>148</v>
       </c>
       <c r="G20" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="29" t="s">
-        <v>231</v>
+      <c r="A21" s="27" t="s">
+        <v>227</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -6048,12 +6289,12 @@
         <v>222</v>
       </c>
       <c r="G21" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="29" t="s">
-        <v>232</v>
+      <c r="A22" s="27" t="s">
+        <v>228</v>
       </c>
       <c r="B22">
         <v>10</v>
@@ -6068,8 +6309,8 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="G22" s="32" t="s">
-        <v>234</v>
+      <c r="G22" s="30" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -6077,8 +6318,8 @@
       <c r="D23" s="9"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="28" t="s">
-        <v>213</v>
+      <c r="A25" s="26" t="s">
+        <v>209</v>
       </c>
       <c r="E25" t="e">
         <f t="shared" si="0"/>
@@ -6086,8 +6327,8 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="28" t="s">
-        <v>219</v>
+      <c r="A26" s="26" t="s">
+        <v>215</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -6095,7 +6336,7 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="27">
+      <c r="D26" s="25">
         <v>3000</v>
       </c>
       <c r="E26">
@@ -6104,8 +6345,8 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29" t="s">
-        <v>215</v>
+      <c r="A27" s="27" t="s">
+        <v>211</v>
       </c>
       <c r="B27">
         <v>5</v>
@@ -6122,8 +6363,8 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="29" t="s">
-        <v>217</v>
+      <c r="A28" s="27" t="s">
+        <v>213</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -6140,8 +6381,8 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="29" t="s">
-        <v>216</v>
+      <c r="A29" s="27" t="s">
+        <v>212</v>
       </c>
       <c r="B29">
         <v>5</v>
@@ -6158,8 +6399,8 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="26" t="s">
-        <v>227</v>
+      <c r="A30" s="24" t="s">
+        <v>223</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -6175,12 +6416,12 @@
         <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="30" t="s">
-        <v>230</v>
+      <c r="A31" s="28" t="s">
+        <v>226</v>
       </c>
       <c r="B31">
         <v>10</v>
@@ -6188,7 +6429,7 @@
       <c r="C31">
         <v>20</v>
       </c>
-      <c r="D31" s="27">
+      <c r="D31" s="25">
         <v>40</v>
       </c>
       <c r="E31">
@@ -6197,8 +6438,8 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="30" t="s">
-        <v>213</v>
+      <c r="A32" s="28" t="s">
+        <v>209</v>
       </c>
       <c r="E32" t="e">
         <f t="shared" si="1"/>
@@ -6206,8 +6447,8 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="31" t="s">
-        <v>228</v>
+      <c r="A33" s="29" t="s">
+        <v>224</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -6215,7 +6456,7 @@
       <c r="C33">
         <v>1</v>
       </c>
-      <c r="D33" s="27">
+      <c r="D33" s="25">
         <v>5000</v>
       </c>
       <c r="E33">
@@ -6225,7 +6466,7 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -6233,7 +6474,7 @@
       <c r="C34">
         <v>1</v>
       </c>
-      <c r="D34" s="27">
+      <c r="D34" s="25">
         <v>7500</v>
       </c>
       <c r="E34">

</xml_diff>